<commit_message>
LGDs added to preprocess
</commit_message>
<xml_diff>
--- a/work/preprocess.xlsx
+++ b/work/preprocess.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="149">
   <si>
     <t xml:space="preserve">obs</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">Gc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGDr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGDc</t>
   </si>
   <si>
     <t xml:space="preserve">1991Q1</t>
@@ -874,10 +880,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N105"/>
+  <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="H3:H105 A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -885,7 +891,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.42"/>
@@ -932,10 +938,16 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>134.8</v>
@@ -970,10 +982,18 @@
       <c r="M2" s="0" t="n">
         <v>0.0277274</v>
       </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">K2/J2</f>
+        <v>0.0641480231790508</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <f aca="false">M2/L2</f>
+        <v>0.229912106135987</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>136</v>
@@ -1008,10 +1028,18 @@
       <c r="M3" s="0" t="n">
         <v>0.0277931</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">K3/J3</f>
+        <v>0.0571136906816151</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">M3/L3</f>
+        <v>0.23375189234651</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>137</v>
@@ -1046,10 +1074,18 @@
       <c r="M4" s="0" t="n">
         <v>0.0289403</v>
       </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">K4/J4</f>
+        <v>0.065653213958336</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">M4/L4</f>
+        <v>0.250132238547969</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>138.2</v>
@@ -1084,10 +1120,18 @@
       <c r="M5" s="0" t="n">
         <v>0.0319692</v>
       </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">K5/J5</f>
+        <v>0.0623641198699905</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <f aca="false">M5/L5</f>
+        <v>0.278477351916376</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>139.1</v>
@@ -1122,10 +1166,18 @@
       <c r="M6" s="0" t="n">
         <v>0.0299742</v>
       </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false">K6/J6</f>
+        <v>0.0644186767889636</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">M6/L6</f>
+        <v>0.272989071038251</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>140.1</v>
@@ -1160,10 +1212,18 @@
       <c r="M7" s="0" t="n">
         <v>0.0260266</v>
       </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">K7/J7</f>
+        <v>0.0665814365508527</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">M7/L7</f>
+        <v>0.246931688804554</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>141.1</v>
@@ -1198,10 +1258,18 @@
       <c r="M8" s="0" t="n">
         <v>0.0337844</v>
       </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">K8/J8</f>
+        <v>0.0926457451688447</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">M8/L8</f>
+        <v>0.326104247104247</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>142.3</v>
@@ -1236,10 +1304,18 @@
       <c r="M9" s="0" t="n">
         <v>0.0294025</v>
       </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false">K9/J9</f>
+        <v>0.0900126280848607</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">M9/L9</f>
+        <v>0.301564102564103</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>143.3</v>
@@ -1274,10 +1350,18 @@
       <c r="M10" s="0" t="n">
         <v>0.0238994</v>
       </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">K10/J10</f>
+        <v>0.0738484419989889</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">M10/L10</f>
+        <v>0.269744920993228</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>144.3</v>
@@ -1312,10 +1396,18 @@
       <c r="M11" s="0" t="n">
         <v>0.021557</v>
       </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false">K11/J11</f>
+        <v>0.0912377025215764</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false">M11/L11</f>
+        <v>0.259722891566265</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>145</v>
@@ -1350,10 +1442,18 @@
       <c r="M12" s="0" t="n">
         <v>0.0183645</v>
       </c>
+      <c r="N12" s="0" t="n">
+        <f aca="false">K12/J12</f>
+        <v>0.07423180219628</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <f aca="false">M12/L12</f>
+        <v>0.243238410596026</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>146.3</v>
@@ -1388,10 +1488,18 @@
       <c r="M13" s="0" t="n">
         <v>0.0146246</v>
       </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">K13/J13</f>
+        <v>0.073225548208923</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">M13/L13</f>
+        <v>0.216982195845697</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>147.1</v>
@@ -1426,10 +1534,18 @@
       <c r="M14" s="0" t="n">
         <v>0.014019</v>
       </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">K14/J14</f>
+        <v>0.0724165458094231</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">M14/L14</f>
+        <v>0.229819672131148</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>147.9</v>
@@ -1464,10 +1580,18 @@
       <c r="M15" s="0" t="n">
         <v>0.0112213</v>
       </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">K15/J15</f>
+        <v>0.0735082170486913</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">M15/L15</f>
+        <v>0.205142595978062</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>149.3</v>
@@ -1502,10 +1626,18 @@
       <c r="M16" s="0" t="n">
         <v>0.0091394</v>
       </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">K16/J16</f>
+        <v>0.0594479274685339</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">M16/L16</f>
+        <v>0.188053497942387</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>150.1</v>
@@ -1540,10 +1672,18 @@
       <c r="M17" s="0" t="n">
         <v>0.0082286</v>
       </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">K17/J17</f>
+        <v>0.0714118217437765</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">M17/L17</f>
+        <v>0.189599078341014</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>151.2</v>
@@ -1578,10 +1718,18 @@
       <c r="M18" s="0" t="n">
         <v>0.0074365</v>
       </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">K18/J18</f>
+        <v>0.060841141116216</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <f aca="false">M18/L18</f>
+        <v>0.170954022988506</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>152.4</v>
@@ -1616,10 +1764,18 @@
       <c r="M19" s="0" t="n">
         <v>0.0082311</v>
       </c>
+      <c r="N19" s="0" t="n">
+        <f aca="false">K19/J19</f>
+        <v>0.0555285938508055</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">M19/L19</f>
+        <v>0.201249388753056</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>153.1</v>
@@ -1654,10 +1810,18 @@
       <c r="M20" s="0" t="n">
         <v>0.0056415</v>
       </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">K20/J20</f>
+        <v>0.058131688126228</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <f aca="false">M20/L20</f>
+        <v>0.146532467532468</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>153.9</v>
@@ -1692,10 +1856,18 @@
       <c r="M21" s="0" t="n">
         <v>0.0047097</v>
       </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">K21/J21</f>
+        <v>0.0490326478447775</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">M21/L21</f>
+        <v>0.137309037900875</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>155.5</v>
@@ -1730,10 +1902,18 @@
       <c r="M22" s="0" t="n">
         <v>0.0047465</v>
       </c>
+      <c r="N22" s="0" t="n">
+        <f aca="false">K22/J22</f>
+        <v>0.0534582046060136</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <f aca="false">M22/L22</f>
+        <v>0.141686567164179</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>156.7</v>
@@ -1768,10 +1948,18 @@
       <c r="M23" s="0" t="n">
         <v>0.003828</v>
       </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">K23/J23</f>
+        <v>0.0433050159089175</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <f aca="false">M23/L23</f>
+        <v>0.119625</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>157.7</v>
@@ -1806,10 +1994,18 @@
       <c r="M24" s="0" t="n">
         <v>0.0036411</v>
       </c>
+      <c r="N24" s="0" t="n">
+        <f aca="false">K24/J24</f>
+        <v>0.04333827631573</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <f aca="false">M24/L24</f>
+        <v>0.117834951456311</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>159.1</v>
@@ -1844,10 +2040,18 @@
       <c r="M25" s="0" t="n">
         <v>0.0025673</v>
       </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">K25/J25</f>
+        <v>0.0342520150098808</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <f aca="false">M25/L25</f>
+        <v>0.0894529616724739</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>159.8</v>
@@ -1882,10 +2086,18 @@
       <c r="M26" s="0" t="n">
         <v>0.0024777</v>
       </c>
+      <c r="N26" s="0" t="n">
+        <f aca="false">K26/J26</f>
+        <v>0.0423593161071526</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <f aca="false">M26/L26</f>
+        <v>0.0942091254752852</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>160.2</v>
@@ -1920,10 +2132,18 @@
       <c r="M27" s="0" t="n">
         <v>0.0019881</v>
       </c>
+      <c r="N27" s="0" t="n">
+        <f aca="false">K27/J27</f>
+        <v>0.0430006010016695</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <f aca="false">M27/L27</f>
+        <v>0.08318410041841</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>161.2</v>
@@ -1958,10 +2178,18 @@
       <c r="M28" s="0" t="n">
         <v>0.0018933</v>
       </c>
+      <c r="N28" s="0" t="n">
+        <f aca="false">K28/J28</f>
+        <v>0.0393049935886689</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <f aca="false">M28/L28</f>
+        <v>0.0834052863436123</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>161.8</v>
@@ -1999,10 +2227,18 @@
       <c r="M29" s="0" t="n">
         <v>0.0017617</v>
       </c>
+      <c r="N29" s="0" t="n">
+        <f aca="false">K29/J29</f>
+        <v>0.0355199467716448</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <f aca="false">M29/L29</f>
+        <v>0.079</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>162</v>
@@ -2040,10 +2276,18 @@
       <c r="M30" s="0" t="n">
         <v>0.0019906</v>
       </c>
+      <c r="N30" s="0" t="n">
+        <f aca="false">K30/J30</f>
+        <v>0.0408374263608237</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <f aca="false">M30/L30</f>
+        <v>0.093018691588785</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>162.8</v>
@@ -2081,10 +2325,18 @@
       <c r="M31" s="0" t="n">
         <v>0.0015116</v>
       </c>
+      <c r="N31" s="0" t="n">
+        <f aca="false">K31/J31</f>
+        <v>0.0366218906185109</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <f aca="false">M31/L31</f>
+        <v>0.0740980392156863</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>163.5</v>
@@ -2122,10 +2374,18 @@
       <c r="M32" s="0" t="n">
         <v>0.0016563</v>
       </c>
+      <c r="N32" s="0" t="n">
+        <f aca="false">K32/J32</f>
+        <v>0.0366419083736708</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <f aca="false">M32/L32</f>
+        <v>0.0840761421319797</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>164.4</v>
@@ -2163,10 +2423,18 @@
       <c r="M33" s="0" t="n">
         <v>0.0017879</v>
       </c>
+      <c r="N33" s="0" t="n">
+        <f aca="false">K33/J33</f>
+        <v>0.0338011760511396</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <f aca="false">M33/L33</f>
+        <v>0.0889502487562189</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>164.8</v>
@@ -2204,10 +2472,18 @@
       <c r="M34" s="0" t="n">
         <v>0.0016852</v>
       </c>
+      <c r="N34" s="0" t="n">
+        <f aca="false">K34/J34</f>
+        <v>0.0512915371902595</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <f aca="false">M34/L34</f>
+        <v>0.0896382978723404</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>166</v>
@@ -2245,10 +2521,18 @@
       <c r="M35" s="0" t="n">
         <v>0.0017457</v>
       </c>
+      <c r="N35" s="0" t="n">
+        <f aca="false">K35/J35</f>
+        <v>0.0570653080329042</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <f aca="false">M35/L35</f>
+        <v>0.0953934426229508</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>167.8</v>
@@ -2286,10 +2570,18 @@
       <c r="M36" s="0" t="n">
         <v>0.0016403</v>
       </c>
+      <c r="N36" s="0" t="n">
+        <f aca="false">K36/J36</f>
+        <v>0.0674157303370787</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <f aca="false">M36/L36</f>
+        <v>0.104477707006369</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>168.8</v>
@@ -2327,10 +2619,18 @@
       <c r="M37" s="0" t="n">
         <v>0.0014534</v>
       </c>
+      <c r="N37" s="0" t="n">
+        <f aca="false">K37/J37</f>
+        <v>0.0664905900777745</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <f aca="false">M37/L37</f>
+        <v>0.0995479452054794</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>171</v>
@@ -2368,10 +2668,18 @@
       <c r="M38" s="0" t="n">
         <v>0.0015929</v>
       </c>
+      <c r="N38" s="0" t="n">
+        <f aca="false">K38/J38</f>
+        <v>0.0655366549835247</v>
+      </c>
+      <c r="O38" s="0" t="n">
+        <f aca="false">M38/L38</f>
+        <v>0.105490066225166</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>172.2</v>
@@ -2409,10 +2717,18 @@
       <c r="M39" s="0" t="n">
         <v>0.0017376</v>
       </c>
+      <c r="N39" s="0" t="n">
+        <f aca="false">K39/J39</f>
+        <v>0.0545407484482821</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <f aca="false">M39/L39</f>
+        <v>0.120666666666667</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>173.6</v>
@@ -2450,10 +2766,18 @@
       <c r="M40" s="0" t="n">
         <v>0.0017692</v>
       </c>
+      <c r="N40" s="0" t="n">
+        <f aca="false">K40/J40</f>
+        <v>0.0609454163546721</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <f aca="false">M40/L40</f>
+        <v>0.119540540540541</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>174.6</v>
@@ -2491,10 +2815,18 @@
       <c r="M41" s="0" t="n">
         <v>0.0018008</v>
       </c>
+      <c r="N41" s="0" t="n">
+        <f aca="false">K41/J41</f>
+        <v>0.0614114622408461</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <f aca="false">M41/L41</f>
+        <v>0.118473684210526</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>176.1</v>
@@ -2532,10 +2864,18 @@
       <c r="M42" s="0" t="n">
         <v>0.002264</v>
       </c>
+      <c r="N42" s="0" t="n">
+        <f aca="false">K42/J42</f>
+        <v>0.0613337452354884</v>
+      </c>
+      <c r="O42" s="0" t="n">
+        <f aca="false">M42/L42</f>
+        <v>0.1415</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>177.7</v>
@@ -2573,10 +2913,18 @@
       <c r="M43" s="0" t="n">
         <v>0.0023667</v>
       </c>
+      <c r="N43" s="0" t="n">
+        <f aca="false">K43/J43</f>
+        <v>0.0659285285799983</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <f aca="false">M43/L43</f>
+        <v>0.136803468208092</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>178.1</v>
@@ -2614,10 +2962,18 @@
       <c r="M44" s="0" t="n">
         <v>0.0028168</v>
       </c>
+      <c r="N44" s="0" t="n">
+        <f aca="false">K44/J44</f>
+        <v>0.201052094447279</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <f aca="false">M44/L44</f>
+        <v>0.146708333333333</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>177.4</v>
@@ -2655,10 +3011,18 @@
       <c r="M45" s="0" t="n">
         <v>0.0032247</v>
       </c>
+      <c r="N45" s="0" t="n">
+        <f aca="false">K45/J45</f>
+        <v>0.0850082311033399</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <f aca="false">M45/L45</f>
+        <v>0.167082901554404</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>178.5</v>
@@ -2696,10 +3060,18 @@
       <c r="M46" s="0" t="n">
         <v>0.0030062</v>
       </c>
+      <c r="N46" s="0" t="n">
+        <f aca="false">K46/J46</f>
+        <v>0.0715687185731149</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <f aca="false">M46/L46</f>
+        <v>0.168887640449438</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>179.6</v>
@@ -2737,10 +3109,18 @@
       <c r="M47" s="0" t="n">
         <v>0.0027904</v>
       </c>
+      <c r="N47" s="0" t="n">
+        <f aca="false">K47/J47</f>
+        <v>0.0782468389990444</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <f aca="false">M47/L47</f>
+        <v>0.158545454545455</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>180.8</v>
@@ -2778,10 +3158,18 @@
       <c r="M48" s="0" t="n">
         <v>0.0027351</v>
       </c>
+      <c r="N48" s="0" t="n">
+        <f aca="false">K48/J48</f>
+        <v>0.070720518966595</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <f aca="false">M48/L48</f>
+        <v>0.161840236686391</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>181.8</v>
@@ -2819,10 +3207,18 @@
       <c r="M49" s="0" t="n">
         <v>0.0027719</v>
       </c>
+      <c r="N49" s="0" t="n">
+        <f aca="false">K49/J49</f>
+        <v>0.0710711716667372</v>
+      </c>
+      <c r="O49" s="0" t="n">
+        <f aca="false">M49/L49</f>
+        <v>0.172167701863354</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>183.9</v>
@@ -2860,10 +3256,18 @@
       <c r="M50" s="0" t="n">
         <v>0.0025193</v>
       </c>
+      <c r="N50" s="0" t="n">
+        <f aca="false">K50/J50</f>
+        <v>0.0753208706088287</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <f aca="false">M50/L50</f>
+        <v>0.15085628742515</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>183.1</v>
@@ -2901,10 +3305,18 @@
       <c r="M51" s="0" t="n">
         <v>0.0027719</v>
       </c>
+      <c r="N51" s="0" t="n">
+        <f aca="false">K51/J51</f>
+        <v>0.0820568703658391</v>
+      </c>
+      <c r="O51" s="0" t="n">
+        <f aca="false">M51/L51</f>
+        <v>0.172167701863354</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>185.1</v>
@@ -2942,10 +3354,18 @@
       <c r="M52" s="0" t="n">
         <v>0.0025692</v>
       </c>
+      <c r="N52" s="0" t="n">
+        <f aca="false">K52/J52</f>
+        <v>0.0749061168484148</v>
+      </c>
+      <c r="O52" s="0" t="n">
+        <f aca="false">M52/L52</f>
+        <v>0.173594594594595</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>185.5</v>
@@ -2983,10 +3403,18 @@
       <c r="M53" s="0" t="n">
         <v>0.002106</v>
       </c>
+      <c r="N53" s="0" t="n">
+        <f aca="false">K53/J53</f>
+        <v>0.190414025922536</v>
+      </c>
+      <c r="O53" s="0" t="n">
+        <f aca="false">M53/L53</f>
+        <v>0.150428571428571</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>187.1</v>
@@ -3024,10 +3452,18 @@
       <c r="M54" s="0" t="n">
         <v>0.0018875</v>
       </c>
+      <c r="N54" s="0" t="n">
+        <f aca="false">K54/J54</f>
+        <v>0.0784735257435846</v>
+      </c>
+      <c r="O54" s="0" t="n">
+        <f aca="false">M54/L54</f>
+        <v>0.151</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>188.9</v>
@@ -3065,10 +3501,18 @@
       <c r="M55" s="0" t="n">
         <v>0.0016954</v>
       </c>
+      <c r="N55" s="0" t="n">
+        <f aca="false">K55/J55</f>
+        <v>0.0687439428136566</v>
+      </c>
+      <c r="O55" s="0" t="n">
+        <f aca="false">M55/L55</f>
+        <v>0.134555555555556</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>189.8</v>
@@ -3106,10 +3550,18 @@
       <c r="M56" s="0" t="n">
         <v>0.0015401</v>
       </c>
+      <c r="N56" s="0" t="n">
+        <f aca="false">K56/J56</f>
+        <v>0.056721859545005</v>
+      </c>
+      <c r="O56" s="0" t="n">
+        <f aca="false">M56/L56</f>
+        <v>0.129420168067227</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>191.7</v>
@@ -3147,10 +3599,18 @@
       <c r="M57" s="0" t="n">
         <v>0.001469</v>
       </c>
+      <c r="N57" s="0" t="n">
+        <f aca="false">K57/J57</f>
+        <v>0.0646475014037058</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <f aca="false">M57/L57</f>
+        <v>0.133545454545455</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>193.1</v>
@@ -3188,10 +3648,18 @@
       <c r="M58" s="0" t="n">
         <v>0.0014848</v>
       </c>
+      <c r="N58" s="0" t="n">
+        <f aca="false">K58/J58</f>
+        <v>0.0558833752672377</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <f aca="false">M58/L58</f>
+        <v>0.132571428571429</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>193.7</v>
@@ -3229,10 +3697,18 @@
       <c r="M59" s="0" t="n">
         <v>0.0013295</v>
       </c>
+      <c r="N59" s="0" t="n">
+        <f aca="false">K59/J59</f>
+        <v>0.0514279563816405</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <f aca="false">M59/L59</f>
+        <v>0.126619047619048</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>198.8</v>
@@ -3270,10 +3746,18 @@
       <c r="M60" s="0" t="n">
         <v>0.0014453</v>
       </c>
+      <c r="N60" s="0" t="n">
+        <f aca="false">K60/J60</f>
+        <v>0.0507562172557862</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <f aca="false">M60/L60</f>
+        <v>0.13507476635514</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>198.1</v>
@@ -3311,10 +3795,18 @@
       <c r="M61" s="0" t="n">
         <v>0.0009137</v>
       </c>
+      <c r="N61" s="0" t="n">
+        <f aca="false">K61/J61</f>
+        <v>0.0427768709470489</v>
+      </c>
+      <c r="O61" s="0" t="n">
+        <f aca="false">M61/L61</f>
+        <v>0.0887087378640777</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>199.7</v>
@@ -3352,10 +3844,18 @@
       <c r="M62" s="0" t="n">
         <v>0.0013058</v>
       </c>
+      <c r="N62" s="0" t="n">
+        <f aca="false">K62/J62</f>
+        <v>0.0559571559686774</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <f aca="false">M62/L62</f>
+        <v>0.128019607843137</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>201.8</v>
@@ -3393,10 +3893,18 @@
       <c r="M63" s="0" t="n">
         <v>0.0011058</v>
       </c>
+      <c r="N63" s="0" t="n">
+        <f aca="false">K63/J63</f>
+        <v>0.0557586506582548</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <f aca="false">M63/L63</f>
+        <v>0.108411764705882</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>202.8</v>
@@ -3434,10 +3942,18 @@
       <c r="M64" s="0" t="n">
         <v>0.0015927</v>
       </c>
+      <c r="N64" s="0" t="n">
+        <f aca="false">K64/J64</f>
+        <v>0.056992315287344</v>
+      </c>
+      <c r="O64" s="0" t="n">
+        <f aca="false">M64/L64</f>
+        <v>0.140946902654867</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>203.1</v>
@@ -3475,10 +3991,18 @@
       <c r="M65" s="0" t="n">
         <v>0.0015428</v>
       </c>
+      <c r="N65" s="0" t="n">
+        <f aca="false">K65/J65</f>
+        <v>0.0612143860993995</v>
+      </c>
+      <c r="O65" s="0" t="n">
+        <f aca="false">M65/L65</f>
+        <v>0.116878787878788</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>205.288</v>
@@ -3516,10 +4040,18 @@
       <c r="M66" s="0" t="n">
         <v>0.0024297</v>
       </c>
+      <c r="N66" s="0" t="n">
+        <f aca="false">K66/J66</f>
+        <v>0.0737720139740321</v>
+      </c>
+      <c r="O66" s="0" t="n">
+        <f aca="false">M66/L66</f>
+        <v>0.169909090909091</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>207.234</v>
@@ -3557,10 +4089,18 @@
       <c r="M67" s="0" t="n">
         <v>0.0023877</v>
       </c>
+      <c r="N67" s="0" t="n">
+        <f aca="false">K67/J67</f>
+        <v>0.0826776027858198</v>
+      </c>
+      <c r="O67" s="0" t="n">
+        <f aca="false">M67/L67</f>
+        <v>0.146484662576687</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>208.547</v>
@@ -3598,10 +4138,18 @@
       <c r="M68" s="0" t="n">
         <v>0.0036563</v>
       </c>
+      <c r="N68" s="0" t="n">
+        <f aca="false">K68/J68</f>
+        <v>0.090775525875958</v>
+      </c>
+      <c r="O68" s="0" t="n">
+        <f aca="false">M68/L68</f>
+        <v>0.185598984771574</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>211.445</v>
@@ -3639,10 +4187,18 @@
       <c r="M69" s="0" t="n">
         <v>0.0048725</v>
       </c>
+      <c r="N69" s="0" t="n">
+        <f aca="false">K69/J69</f>
+        <v>0.145639623930818</v>
+      </c>
+      <c r="O69" s="0" t="n">
+        <f aca="false">M69/L69</f>
+        <v>0.177181818181818</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>213.448</v>
@@ -3680,10 +4236,18 @@
       <c r="M70" s="0" t="n">
         <v>0.0088729</v>
       </c>
+      <c r="N70" s="0" t="n">
+        <f aca="false">K70/J70</f>
+        <v>0.230145340201447</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <f aca="false">M70/L70</f>
+        <v>0.252789173789174</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>217.463</v>
@@ -3721,10 +4285,18 @@
       <c r="M71" s="0" t="n">
         <v>0.0127864</v>
       </c>
+      <c r="N71" s="0" t="n">
+        <f aca="false">K71/J71</f>
+        <v>0.266234531526223</v>
+      </c>
+      <c r="O71" s="0" t="n">
+        <f aca="false">M71/L71</f>
+        <v>0.307365384615385</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>218.877</v>
@@ -3762,10 +4334,18 @@
       <c r="M72" s="0" t="n">
         <v>0.0149656</v>
       </c>
+      <c r="N72" s="0" t="n">
+        <f aca="false">K72/J72</f>
+        <v>0.315777930143274</v>
+      </c>
+      <c r="O72" s="0" t="n">
+        <f aca="false">M72/L72</f>
+        <v>0.322534482758621</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>211.398</v>
@@ -3803,10 +4383,18 @@
       <c r="M73" s="0" t="n">
         <v>0.0242371</v>
       </c>
+      <c r="N73" s="0" t="n">
+        <f aca="false">K73/J73</f>
+        <v>0.243495004968717</v>
+      </c>
+      <c r="O73" s="0" t="n">
+        <f aca="false">M73/L73</f>
+        <v>0.44147723132969</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>212.495</v>
@@ -3844,10 +4432,18 @@
       <c r="M74" s="0" t="n">
         <v>0.0209061</v>
       </c>
+      <c r="N74" s="0" t="n">
+        <f aca="false">K74/J74</f>
+        <v>0.231730360989826</v>
+      </c>
+      <c r="O74" s="0" t="n">
+        <f aca="false">M74/L74</f>
+        <v>0.317239757207891</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>214.79</v>
@@ -3885,10 +4481,18 @@
       <c r="M75" s="0" t="n">
         <v>0.0291015</v>
       </c>
+      <c r="N75" s="0" t="n">
+        <f aca="false">K75/J75</f>
+        <v>0.269261674444479</v>
+      </c>
+      <c r="O75" s="0" t="n">
+        <f aca="false">M75/L75</f>
+        <v>0.37071974522293</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>215.861</v>
@@ -3926,10 +4530,18 @@
       <c r="M76" s="0" t="n">
         <v>0.032115</v>
       </c>
+      <c r="N76" s="0" t="n">
+        <f aca="false">K76/J76</f>
+        <v>0.250939791309632</v>
+      </c>
+      <c r="O76" s="0" t="n">
+        <f aca="false">M76/L76</f>
+        <v>0.377823529411765</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>217.347</v>
@@ -3967,10 +4579,18 @@
       <c r="M77" s="0" t="n">
         <v>0.0362967</v>
       </c>
+      <c r="N77" s="0" t="n">
+        <f aca="false">K77/J77</f>
+        <v>0.262872465485917</v>
+      </c>
+      <c r="O77" s="0" t="n">
+        <f aca="false">M77/L77</f>
+        <v>0.415769759450172</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>217.353</v>
@@ -4008,10 +4628,18 @@
       <c r="M78" s="0" t="n">
         <v>0.0309204</v>
       </c>
+      <c r="N78" s="0" t="n">
+        <f aca="false">K78/J78</f>
+        <v>0.218416943551755</v>
+      </c>
+      <c r="O78" s="0" t="n">
+        <f aca="false">M78/L78</f>
+        <v>0.352972602739726</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>217.199</v>
@@ -4049,10 +4677,18 @@
       <c r="M79" s="0" t="n">
         <v>0.0309283</v>
       </c>
+      <c r="N79" s="0" t="n">
+        <f aca="false">K79/J79</f>
+        <v>0.19312025107367</v>
+      </c>
+      <c r="O79" s="0" t="n">
+        <f aca="false">M79/L79</f>
+        <v>0.352660205245154</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>218.275</v>
@@ -4090,10 +4726,18 @@
       <c r="M80" s="0" t="n">
         <v>0.030194</v>
       </c>
+      <c r="N80" s="0" t="n">
+        <f aca="false">K80/J80</f>
+        <v>0.177459693499687</v>
+      </c>
+      <c r="O80" s="0" t="n">
+        <f aca="false">M80/L80</f>
+        <v>0.351093023255814</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>220.472</v>
@@ -4131,10 +4775,18 @@
       <c r="M81" s="0" t="n">
         <v>0.0276884</v>
       </c>
+      <c r="N81" s="0" t="n">
+        <f aca="false">K81/J81</f>
+        <v>0.19287883141235</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <f aca="false">M81/L81</f>
+        <v>0.347844221105528</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>223.044</v>
@@ -4172,10 +4824,18 @@
       <c r="M82" s="0" t="n">
         <v>0.0238724</v>
       </c>
+      <c r="N82" s="0" t="n">
+        <f aca="false">K82/J82</f>
+        <v>0.165295791229275</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <f aca="false">M82/L82</f>
+        <v>0.315772486772487</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>224.841</v>
@@ -4213,10 +4873,18 @@
       <c r="M83" s="0" t="n">
         <v>0.0205011</v>
       </c>
+      <c r="N83" s="0" t="n">
+        <f aca="false">K83/J83</f>
+        <v>0.158581476686441</v>
+      </c>
+      <c r="O83" s="0" t="n">
+        <f aca="false">M83/L83</f>
+        <v>0.28915514809591</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>226.676</v>
@@ -4254,10 +4922,18 @@
       <c r="M84" s="0" t="n">
         <v>0.0177614</v>
       </c>
+      <c r="N84" s="0" t="n">
+        <f aca="false">K84/J84</f>
+        <v>0.146499645334174</v>
+      </c>
+      <c r="O84" s="0" t="n">
+        <f aca="false">M84/L84</f>
+        <v>0.266687687687688</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>227.145</v>
@@ -4295,10 +4971,18 @@
       <c r="M85" s="0" t="n">
         <v>0.0159348</v>
       </c>
+      <c r="N85" s="0" t="n">
+        <f aca="false">K85/J85</f>
+        <v>0.134015877578124</v>
+      </c>
+      <c r="O85" s="0" t="n">
+        <f aca="false">M85/L85</f>
+        <v>0.260372549019608</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>228.866</v>
@@ -4336,10 +5020,18 @@
       <c r="M86" s="0" t="n">
         <v>0.0138292</v>
       </c>
+      <c r="N86" s="0" t="n">
+        <f aca="false">K86/J86</f>
+        <v>0.135214726356336</v>
+      </c>
+      <c r="O86" s="0" t="n">
+        <f aca="false">M86/L86</f>
+        <v>0.252357664233577</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>228.626</v>
@@ -4377,10 +5069,18 @@
       <c r="M87" s="0" t="n">
         <v>0.01185</v>
       </c>
+      <c r="N87" s="0" t="n">
+        <f aca="false">K87/J87</f>
+        <v>0.119147877498854</v>
+      </c>
+      <c r="O87" s="0" t="n">
+        <f aca="false">M87/L87</f>
+        <v>0.237</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>231.104</v>
@@ -4418,10 +5118,18 @@
       <c r="M88" s="0" t="n">
         <v>0.0102419</v>
       </c>
+      <c r="N88" s="0" t="n">
+        <f aca="false">K88/J88</f>
+        <v>0.162926666029257</v>
+      </c>
+      <c r="O88" s="0" t="n">
+        <f aca="false">M88/L88</f>
+        <v>0.222167028199566</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>231.165</v>
@@ -4459,10 +5167,18 @@
       <c r="M89" s="0" t="n">
         <v>0.0084706</v>
       </c>
+      <c r="N89" s="0" t="n">
+        <f aca="false">K89/J89</f>
+        <v>0.104501665002174</v>
+      </c>
+      <c r="O89" s="0" t="n">
+        <f aca="false">M89/L89</f>
+        <v>0.204603864734299</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>232.245</v>
@@ -4500,10 +5216,18 @@
       <c r="M90" s="0" t="n">
         <v>0.0075914</v>
       </c>
+      <c r="N90" s="0" t="n">
+        <f aca="false">K90/J90</f>
+        <v>0.0943003467433497</v>
+      </c>
+      <c r="O90" s="0" t="n">
+        <f aca="false">M90/L90</f>
+        <v>0.207415300546448</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>232.583</v>
@@ -4541,10 +5265,18 @@
       <c r="M91" s="0" t="n">
         <v>0.0056991</v>
       </c>
+      <c r="N91" s="0" t="n">
+        <f aca="false">K91/J91</f>
+        <v>0.0806466307378465</v>
+      </c>
+      <c r="O91" s="0" t="n">
+        <f aca="false">M91/L91</f>
+        <v>0.173224924012158</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>233.773</v>
@@ -4582,10 +5314,18 @@
       <c r="M92" s="0" t="n">
         <v>0.0042278</v>
       </c>
+      <c r="N92" s="0" t="n">
+        <f aca="false">K92/J92</f>
+        <v>0.0554792697225433</v>
+      </c>
+      <c r="O92" s="0" t="n">
+        <f aca="false">M92/L92</f>
+        <v>0.149921985815603</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>234.697</v>
@@ -4623,10 +5363,18 @@
       <c r="M93" s="0" t="n">
         <v>0.0029513</v>
       </c>
+      <c r="N93" s="0" t="n">
+        <f aca="false">K93/J93</f>
+        <v>0.0557262142773139</v>
+      </c>
+      <c r="O93" s="0" t="n">
+        <f aca="false">M93/L93</f>
+        <v>0.119485829959514</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>235.79</v>
@@ -4664,10 +5412,18 @@
       <c r="M94" s="0" t="n">
         <v>0.003138</v>
       </c>
+      <c r="N94" s="0" t="n">
+        <f aca="false">K94/J94</f>
+        <v>0.0472406325530728</v>
+      </c>
+      <c r="O94" s="0" t="n">
+        <f aca="false">M94/L94</f>
+        <v>0.142636363636364</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>237.348</v>
@@ -4705,10 +5461,18 @@
       <c r="M95" s="0" t="n">
         <v>0.0024405</v>
       </c>
+      <c r="N95" s="0" t="n">
+        <f aca="false">K95/J95</f>
+        <v>0.039243784673704</v>
+      </c>
+      <c r="O95" s="0" t="n">
+        <f aca="false">M95/L95</f>
+        <v>0.125153846153846</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>237.626</v>
@@ -4746,10 +5510,18 @@
       <c r="M96" s="0" t="n">
         <v>0.0018983</v>
       </c>
+      <c r="N96" s="0" t="n">
+        <f aca="false">K96/J96</f>
+        <v>0.0369697785870911</v>
+      </c>
+      <c r="O96" s="0" t="n">
+        <f aca="false">M96/L96</f>
+        <v>0.107248587570621</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>236.284</v>
@@ -4787,10 +5559,18 @@
       <c r="M97" s="0" t="n">
         <v>0.0013482</v>
       </c>
+      <c r="N97" s="0" t="n">
+        <f aca="false">K97/J97</f>
+        <v>0.0361865815289234</v>
+      </c>
+      <c r="O97" s="0" t="n">
+        <f aca="false">M97/L97</f>
+        <v>0.0853291139240506</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>235.989</v>
@@ -4828,10 +5608,18 @@
       <c r="M98" s="0" t="n">
         <v>0.0024</v>
       </c>
+      <c r="N98" s="0" t="n">
+        <f aca="false">K98/J98</f>
+        <v>0.043338683788122</v>
+      </c>
+      <c r="O98" s="0" t="n">
+        <f aca="false">M98/L98</f>
+        <v>0.170212765957447</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>237.419</v>
@@ -4870,12 +5658,17 @@
         <v>0.0003</v>
       </c>
       <c r="N99" s="0" t="n">
-        <v>0.0003</v>
+        <f aca="false">K99/J99</f>
+        <v>0.0362068965517241</v>
+      </c>
+      <c r="O99" s="0" t="n">
+        <f aca="false">M99/L99</f>
+        <v>0.0236220472440945</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>237.467</v>
@@ -4914,12 +5707,17 @@
         <v>0.0001</v>
       </c>
       <c r="N100" s="0" t="n">
-        <v>-0.0008</v>
+        <f aca="false">K100/J100</f>
+        <v>0.0277777777777778</v>
+      </c>
+      <c r="O100" s="0" t="n">
+        <f aca="false">M100/L100</f>
+        <v>0.00862068965517241</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>237.846</v>
@@ -4958,12 +5756,17 @@
         <v>0.0001</v>
       </c>
       <c r="N101" s="0" t="n">
-        <v>-0.0006</v>
+        <f aca="false">K101/J101</f>
+        <v>0.0392927308447937</v>
+      </c>
+      <c r="O101" s="0" t="n">
+        <f aca="false">M101/L101</f>
+        <v>0.00943396226415094</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>238.078</v>
@@ -5002,12 +5805,17 @@
         <v>0.0001</v>
       </c>
       <c r="N102" s="0" t="n">
-        <v>-0.0001</v>
+        <f aca="false">K102/J102</f>
+        <v>0.027027027027027</v>
+      </c>
+      <c r="O102" s="0" t="n">
+        <f aca="false">M102/L102</f>
+        <v>0.0103092783505155</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>239.842</v>
@@ -5046,12 +5854,17 @@
         <v>0.0001</v>
       </c>
       <c r="N103" s="0" t="n">
-        <v>-0.0001</v>
+        <f aca="false">K103/J103</f>
+        <v>0.0240700218818381</v>
+      </c>
+      <c r="O103" s="0" t="n">
+        <f aca="false">M103/L103</f>
+        <v>0.0108695652173913</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>241.006</v>
@@ -5090,12 +5903,17 @@
         <v>0.0002</v>
       </c>
       <c r="N104" s="0" t="n">
-        <v>0.0002</v>
+        <f aca="false">K104/J104</f>
+        <v>0.0229357798165138</v>
+      </c>
+      <c r="O104" s="0" t="n">
+        <f aca="false">M104/L104</f>
+        <v>0.0229885057471264</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>242.821</v>
@@ -5134,7 +5952,12 @@
         <v>0.0001</v>
       </c>
       <c r="N105" s="0" t="n">
-        <v>0.0001</v>
+        <f aca="false">K105/J105</f>
+        <v>0.0168674698795181</v>
+      </c>
+      <c r="O105" s="0" t="n">
+        <f aca="false">M105/L105</f>
+        <v>0.0117647058823529</v>
       </c>
     </row>
   </sheetData>
@@ -5155,8 +5978,8 @@
   </sheetPr>
   <dimension ref="A2:B97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="H3:H105 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6138,8 +6961,8 @@
   </sheetPr>
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="H3:H105 B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6149,10 +6972,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6939,8 +7762,8 @@
   </sheetPr>
   <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="H3:H105 B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6950,19 +7773,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">VAR('HPIc comp'!B3:B78)</f>
         <v>0.0014725543108307</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">SQRT(B3)</f>
@@ -6971,7 +7794,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.96</v>
@@ -6979,7 +7802,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -7103,7 +7926,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">$B$4^B6</f>
@@ -7228,7 +8051,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7/SUM($B$7:$AE$7)</f>
@@ -7353,7 +8176,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">$B$3*B6*B8</f>
@@ -7478,7 +8301,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">SUM(B9:AE9)</f>
@@ -7487,7 +8310,7 @@
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B11" s="2" t="n">
         <f aca="false">SQRT(B10)</f>
@@ -7496,19 +8319,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">VAR('HPIr comp'!B:B)</f>
         <v>0.000254469046942981</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">SQRT(B15)</f>
@@ -7517,7 +8340,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.96</v>
@@ -7525,7 +8348,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -7649,7 +8472,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">$B$16^B18</f>
@@ -7774,7 +8597,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">B19/SUM($B$7:$AE$7)</f>
@@ -7899,7 +8722,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">$B$15*B18*B20</f>
@@ -8024,7 +8847,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">SUM(B21:AE21)</f>
@@ -8033,7 +8856,7 @@
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2" t="n">
         <f aca="false">SQRT(B22)</f>
@@ -8058,8 +8881,8 @@
   </sheetPr>
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3:H105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8074,21 +8897,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">SUM(E:E)</f>
@@ -8155,7 +8978,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">SUM(G:G)</f>
@@ -8222,7 +9045,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">Input!A8</f>
@@ -8245,7 +9068,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">Input!A9</f>
@@ -8268,7 +9091,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">Input!A10</f>
@@ -8311,7 +9134,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">Input!A12</f>
@@ -8334,7 +9157,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">Input!A13</f>
@@ -8357,7 +9180,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">Input!A14</f>
@@ -8380,7 +9203,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">Input!A15</f>
@@ -8403,7 +9226,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">Input!A16</f>
@@ -10222,8 +11045,8 @@
   </sheetPr>
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="H3:H105 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10233,10 +11056,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11297,8 +12120,8 @@
   </sheetPr>
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H58" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L58" activeCellId="1" sqref="H3:H105 L58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11339,16 +12162,16 @@
         <v>FEDR</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
sent to P for forecasts
</commit_message>
<xml_diff>
--- a/work/preprocess.xlsx
+++ b/work/preprocess.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Input - history" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Input - forecasts" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Input - forecast" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="HPIr comp" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="HPIc comp" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="rhos computation" sheetId="5" state="visible" r:id="rId6"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
   <si>
     <t xml:space="preserve">obs</t>
   </si>
@@ -415,6 +415,18 @@
     <t xml:space="preserve">2016Q4</t>
   </si>
   <si>
+    <t xml:space="preserve">2017Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017Q4</t>
+  </si>
+  <si>
     <t xml:space="preserve">log</t>
   </si>
   <si>
@@ -503,18 +515,6 @@
   </si>
   <si>
     <t xml:space="preserve">Yc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017Q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017Q4</t>
   </si>
 </sst>
 </file>
@@ -907,7 +907,7 @@
   <dimension ref="A1:O105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6000,10 +6000,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6040,13 +6040,113 @@
         <f aca="false">'Input - history'!G1</f>
         <v>HPIr</v>
       </c>
-      <c r="H1" s="0" t="str">
-        <f aca="false">'Input - history'!H1</f>
-        <v>HPIc</v>
-      </c>
       <c r="I1" s="2" t="str">
         <f aca="false">'Input - history'!I1</f>
         <v>FEDR</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>242.821</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>16889.1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>16266.8</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>104.438</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>185.54</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>242.821</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>16889.1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>16266.8</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>104.438</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>185.54</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>242.821</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>16889.1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>16266.8</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>104.438</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>185.54</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>242.821</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>16889.1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>16266.8</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>104.438</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>185.54</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.54</v>
       </c>
     </row>
   </sheetData>
@@ -7061,10 +7161,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7862,19 +7962,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">VAR('HPIc comp'!B3:B78)</f>
         <v>0.0014725543108307</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">SQRT(B3)</f>
@@ -7883,7 +7983,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.96</v>
@@ -7891,7 +7991,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -8015,7 +8115,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">$B$4^B6</f>
@@ -8140,7 +8240,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7/SUM($B$7:$AE$7)</f>
@@ -8265,7 +8365,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">$B$3*B6*B8</f>
@@ -8390,7 +8490,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">SUM(B9:AE9)</f>
@@ -8399,7 +8499,7 @@
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B11" s="2" t="n">
         <f aca="false">SQRT(B10)</f>
@@ -8408,19 +8508,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">VAR('HPIr comp'!B:B)</f>
         <v>0.000254469046942981</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">SQRT(B15)</f>
@@ -8429,7 +8529,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.96</v>
@@ -8437,7 +8537,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -8561,7 +8661,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">$B$16^B18</f>
@@ -8686,7 +8786,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">B19/SUM($B$7:$AE$7)</f>
@@ -8811,7 +8911,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B21" s="0" t="n">
         <f aca="false">$B$15*B18*B20</f>
@@ -8936,7 +9036,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">SUM(B21:AE21)</f>
@@ -8945,7 +9045,7 @@
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B23" s="2" t="n">
         <f aca="false">SQRT(B22)</f>
@@ -8986,21 +9086,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">SUM(E:E)</f>
@@ -9067,7 +9167,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">SUM(G:G)</f>
@@ -9134,7 +9234,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C8" s="0" t="str">
         <f aca="false">'Input - history'!A8</f>
@@ -9157,7 +9257,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C9" s="0" t="str">
         <f aca="false">'Input - history'!A9</f>
@@ -9180,7 +9280,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C10" s="0" t="str">
         <f aca="false">'Input - history'!A10</f>
@@ -9223,7 +9323,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C12" s="0" t="str">
         <f aca="false">'Input - history'!A12</f>
@@ -9246,7 +9346,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C13" s="0" t="str">
         <f aca="false">'Input - history'!A13</f>
@@ -9269,7 +9369,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C14" s="0" t="str">
         <f aca="false">'Input - history'!A14</f>
@@ -9292,7 +9392,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C15" s="0" t="str">
         <f aca="false">'Input - history'!A15</f>
@@ -9315,7 +9415,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C16" s="0" t="str">
         <f aca="false">'Input - history'!A16</f>
@@ -11132,10 +11232,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11145,10 +11245,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12188,6 +12288,46 @@
       </c>
       <c r="B105" s="0" t="n">
         <f aca="false">'Input - history'!$B$105/'Input - history'!B105</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="str">
+        <f aca="false">'Input - forecast'!A2</f>
+        <v>2017Q1</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <f aca="false">'Input - history'!$B$105/'Input - forecast'!B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="str">
+        <f aca="false">'Input - forecast'!A3</f>
+        <v>2017Q2</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <f aca="false">'Input - history'!$B$105/'Input - forecast'!B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="str">
+        <f aca="false">'Input - forecast'!A4</f>
+        <v>2017Q3</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <f aca="false">'Input - history'!$B$105/'Input - forecast'!B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="str">
+        <f aca="false">'Input - forecast'!A5</f>
+        <v>2017Q4</v>
+      </c>
+      <c r="B109" s="0" t="n">
+        <f aca="false">'Input - history'!$B$105/'Input - forecast'!B5</f>
         <v>1</v>
       </c>
     </row>
@@ -12209,8 +12349,8 @@
   </sheetPr>
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B107" activeCellId="0" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12251,16 +12391,16 @@
         <v>FEDR</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17465,199 +17605,147 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="B106" s="3" t="n">
-        <f aca="false">B105</f>
+        <f aca="false">IF('Input - forecast'!C2="","",LN('Input - forecast'!C2))</f>
         <v>9.73442372241407</v>
       </c>
       <c r="C106" s="3" t="n">
-        <f aca="false">C105</f>
+        <f aca="false">IF('Input - forecast'!D2="","",LN('Input - forecast'!D2))</f>
         <v>9.69688149986085</v>
       </c>
       <c r="D106" s="3" t="n">
-        <f aca="false">D105</f>
+        <f aca="false">IF('Input - forecast'!E2="","",LN('Input - forecast'!E2))</f>
         <v>1.54756250871601</v>
       </c>
       <c r="E106" s="3" t="n">
-        <f aca="false">E105</f>
+        <f aca="false">IF('Input - forecast'!F2="","",LN('Input - forecast'!F2*Escsount!$B106))</f>
         <v>4.64859359389652</v>
       </c>
       <c r="F106" s="3" t="n">
-        <f aca="false">F105</f>
+        <f aca="false">IF('Input - forecast'!G2="","",LN('Input - forecast'!G2))</f>
         <v>5.22327049222513</v>
       </c>
-      <c r="G106" s="3" t="n">
-        <f aca="false">G105</f>
-        <v>4.84149154470074</v>
+      <c r="G106" s="3" t="str">
+        <f aca="false">IF('Input - forecast'!H2="","",LN('Input - forecast'!H2*Escsount!$B106))</f>
+        <v/>
       </c>
       <c r="H106" s="3" t="n">
-        <f aca="false">H105</f>
+        <f aca="false">IF('Input - forecast'!I2="","",'Input - forecast'!I2)</f>
         <v>0.54</v>
-      </c>
-      <c r="I106" s="3" t="n">
-        <f aca="false">I105</f>
-        <v>1.7335385038418</v>
-      </c>
-      <c r="J106" s="3" t="n">
-        <f aca="false">J105</f>
-        <v>0.0110340402922172</v>
-      </c>
-      <c r="K106" s="3" t="n">
-        <f aca="false">K105</f>
-        <v>2.38670773449225</v>
-      </c>
-      <c r="L106" s="3" t="n">
-        <f aca="false">L105</f>
-        <v>0.128532745950033</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="B107" s="3" t="n">
-        <f aca="false">B106</f>
+        <f aca="false">IF('Input - forecast'!C3="","",LN('Input - forecast'!C3))</f>
         <v>9.73442372241407</v>
       </c>
       <c r="C107" s="3" t="n">
-        <f aca="false">C106</f>
+        <f aca="false">IF('Input - forecast'!D3="","",LN('Input - forecast'!D3))</f>
         <v>9.69688149986085</v>
       </c>
       <c r="D107" s="3" t="n">
-        <f aca="false">D106</f>
+        <f aca="false">IF('Input - forecast'!E3="","",LN('Input - forecast'!E3))</f>
         <v>1.54756250871601</v>
       </c>
       <c r="E107" s="3" t="n">
-        <f aca="false">E106</f>
+        <f aca="false">IF('Input - forecast'!F3="","",LN('Input - forecast'!F3*Escsount!$B107))</f>
         <v>4.64859359389652</v>
       </c>
       <c r="F107" s="3" t="n">
-        <f aca="false">F106</f>
+        <f aca="false">IF('Input - forecast'!G3="","",LN('Input - forecast'!G3))</f>
         <v>5.22327049222513</v>
       </c>
-      <c r="G107" s="3" t="n">
-        <f aca="false">G106</f>
-        <v>4.84149154470074</v>
+      <c r="G107" s="3" t="str">
+        <f aca="false">IF('Input - forecast'!H3="","",LN('Input - forecast'!H3*Escsount!$B107))</f>
+        <v/>
       </c>
       <c r="H107" s="3" t="n">
-        <f aca="false">H106</f>
+        <f aca="false">IF('Input - forecast'!I3="","",'Input - forecast'!I3)</f>
         <v>0.54</v>
       </c>
-      <c r="I107" s="3" t="n">
-        <f aca="false">I106</f>
-        <v>1.7335385038418</v>
-      </c>
-      <c r="J107" s="3" t="n">
-        <f aca="false">J106</f>
-        <v>0.0110340402922172</v>
-      </c>
-      <c r="K107" s="3" t="n">
-        <f aca="false">K106</f>
-        <v>2.38670773449225</v>
-      </c>
-      <c r="L107" s="3" t="n">
-        <f aca="false">L106</f>
-        <v>0.128532745950033</v>
-      </c>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="B108" s="3" t="n">
-        <f aca="false">B107</f>
+        <f aca="false">IF('Input - forecast'!C4="","",LN('Input - forecast'!C4))</f>
         <v>9.73442372241407</v>
       </c>
       <c r="C108" s="3" t="n">
-        <f aca="false">C107</f>
+        <f aca="false">IF('Input - forecast'!D4="","",LN('Input - forecast'!D4))</f>
         <v>9.69688149986085</v>
       </c>
       <c r="D108" s="3" t="n">
-        <f aca="false">D107</f>
+        <f aca="false">IF('Input - forecast'!E4="","",LN('Input - forecast'!E4))</f>
         <v>1.54756250871601</v>
       </c>
       <c r="E108" s="3" t="n">
-        <f aca="false">E107</f>
+        <f aca="false">IF('Input - forecast'!F4="","",LN('Input - forecast'!F4*Escsount!$B108))</f>
         <v>4.64859359389652</v>
       </c>
       <c r="F108" s="3" t="n">
-        <f aca="false">F107</f>
+        <f aca="false">IF('Input - forecast'!G4="","",LN('Input - forecast'!G4))</f>
         <v>5.22327049222513</v>
       </c>
-      <c r="G108" s="3" t="n">
-        <f aca="false">G107</f>
-        <v>4.84149154470074</v>
+      <c r="G108" s="3" t="str">
+        <f aca="false">IF('Input - forecast'!H4="","",LN('Input - forecast'!H4*Escsount!$B108))</f>
+        <v/>
       </c>
       <c r="H108" s="3" t="n">
-        <f aca="false">H107</f>
+        <f aca="false">IF('Input - forecast'!I4="","",'Input - forecast'!I4)</f>
         <v>0.54</v>
       </c>
-      <c r="I108" s="3" t="n">
-        <f aca="false">I107</f>
-        <v>1.7335385038418</v>
-      </c>
-      <c r="J108" s="3" t="n">
-        <f aca="false">J107</f>
-        <v>0.0110340402922172</v>
-      </c>
-      <c r="K108" s="3" t="n">
-        <f aca="false">K107</f>
-        <v>2.38670773449225</v>
-      </c>
-      <c r="L108" s="3" t="n">
-        <f aca="false">L107</f>
-        <v>0.128532745950033</v>
-      </c>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B109" s="3" t="n">
-        <f aca="false">B108</f>
+        <f aca="false">IF('Input - forecast'!C5="","",LN('Input - forecast'!C5))</f>
         <v>9.73442372241407</v>
       </c>
       <c r="C109" s="3" t="n">
-        <f aca="false">C108</f>
+        <f aca="false">IF('Input - forecast'!D5="","",LN('Input - forecast'!D5))</f>
         <v>9.69688149986085</v>
       </c>
       <c r="D109" s="3" t="n">
-        <f aca="false">D108</f>
+        <f aca="false">IF('Input - forecast'!E5="","",LN('Input - forecast'!E5))</f>
         <v>1.54756250871601</v>
       </c>
       <c r="E109" s="3" t="n">
-        <f aca="false">E108</f>
+        <f aca="false">IF('Input - forecast'!F5="","",LN('Input - forecast'!F5*Escsount!$B109))</f>
         <v>4.64859359389652</v>
       </c>
       <c r="F109" s="3" t="n">
-        <f aca="false">F108</f>
+        <f aca="false">IF('Input - forecast'!G5="","",LN('Input - forecast'!G5))</f>
         <v>5.22327049222513</v>
       </c>
-      <c r="G109" s="3" t="n">
-        <f aca="false">G108</f>
-        <v>4.84149154470074</v>
+      <c r="G109" s="3" t="str">
+        <f aca="false">IF('Input - forecast'!H5="","",LN('Input - forecast'!H5*Escsount!$B109))</f>
+        <v/>
       </c>
       <c r="H109" s="3" t="n">
-        <f aca="false">H108</f>
+        <f aca="false">IF('Input - forecast'!I5="","",'Input - forecast'!I5)</f>
         <v>0.54</v>
       </c>
-      <c r="I109" s="3" t="n">
-        <f aca="false">I108</f>
-        <v>1.7335385038418</v>
-      </c>
-      <c r="J109" s="3" t="n">
-        <f aca="false">J108</f>
-        <v>0.0110340402922172</v>
-      </c>
-      <c r="K109" s="3" t="n">
-        <f aca="false">K108</f>
-        <v>2.38670773449225</v>
-      </c>
-      <c r="L109" s="3" t="n">
-        <f aca="false">L108</f>
-        <v>0.128532745950033</v>
-      </c>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>